<commit_message>
moved watchdog reset to polling
</commit_message>
<xml_diff>
--- a/software/projects/MSIExhibit/doc/RobotInfo.xlsx
+++ b/software/projects/MSIExhibit/doc/RobotInfo.xlsx
@@ -44,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +180,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -368,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -483,15 +490,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -537,17 +535,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -892,204 +891,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="14.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="14.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>112</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>142</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>153</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>157</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>158</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>169</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>171</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>128</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>113</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B27" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C27" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>133</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>135</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B29" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>142</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>170</v>
+      </c>
+      <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>153</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>157</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>158</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>160</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D32" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>169</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>170</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>128</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started editing cluster code - stopped because it won't work better than what is already there.
</commit_message>
<xml_diff>
--- a/software/projects/MSIExhibit/doc/RobotInfo.xlsx
+++ b/software/projects/MSIExhibit/doc/RobotInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>robot ID</t>
   </si>
@@ -37,7 +37,22 @@
     <t>twitchy follower</t>
   </si>
   <si>
-    <t>bad fr bump sensor</t>
+    <t>bad bump sensors</t>
+  </si>
+  <si>
+    <t>bad front (right?) bump sensor</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>very twitchy follower</t>
+  </si>
+  <si>
+    <t>Not turning on</t>
+  </si>
+  <si>
+    <t>bad right encoder, bizarre behavior</t>
   </si>
 </sst>
 </file>
@@ -188,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,14 +383,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -490,6 +499,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -535,18 +553,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -594,7 +616,28 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -891,209 +934,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="3" width="14.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="4" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="50.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
         <v>112</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7">
+        <v>113</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>128</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>133</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>135</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
         <v>142</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C11" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1">
         <v>153</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
         <v>157</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1">
         <v>158</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D19" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
         <v>169</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D22" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>170</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" s="3">
         <v>171</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>128</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
-        <v>113</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>97</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1">
+        <v>114</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
+        <v>160</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>133</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>135</v>
-      </c>
-      <c r="B29" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>170</v>
-      </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>160</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>7</v>
+      <c r="B28" s="1">
+        <v>98</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E27">
+    <sortCondition ref="A2:A27"/>
+    <sortCondition ref="B2:B27"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added IIR for battery voltage added 4 sec timer for battery shutdown updated MSP to ver 26
</commit_message>
<xml_diff>
--- a/software/projects/MSIExhibit/doc/RobotInfo.xlsx
+++ b/software/projects/MSIExhibit/doc/RobotInfo.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>robot ID</t>
-  </si>
-  <si>
-    <t>bad radio</t>
   </si>
   <si>
     <t>bad IR</t>
@@ -54,12 +51,30 @@
   <si>
     <t>bad right encoder, bizarre behavior</t>
   </si>
+  <si>
+    <t>bottom board not working</t>
+  </si>
+  <si>
+    <t>updated</t>
+  </si>
+  <si>
+    <t>shut down at 3.84 volts,
+Custom MSP firmware with IIR filter
+3.83v @ 3:54pm</t>
+  </si>
+  <si>
+    <t>custom MSP firmware with IIR filter
+3.73v @ 3:54pm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +217,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -384,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -508,6 +530,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -553,23 +584,32 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -616,24 +656,298 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -934,35 +1248,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="4" width="14.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
+      <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,55 +1285,57 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>110</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>112</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" s="7">
-        <v>113</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="B4" s="1">
+        <v>110</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" s="1">
-        <v>121</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
-        <v>128</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="1">
+        <v>121</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1027,6 +1344,8 @@
       <c r="B7" s="1">
         <v>131</v>
       </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1035,30 +1354,38 @@
       <c r="B8" s="1">
         <v>133</v>
       </c>
-      <c r="D8" s="2">
+      <c r="C8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="11"/>
+      <c r="E8" s="7">
+        <v>42172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1">
         <v>135</v>
       </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
+      <c r="D9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>138</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1069,45 +1396,57 @@
         <v>142</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0</v>
       </c>
       <c r="B12" s="1">
-        <v>143</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>144</v>
+        <v>146</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>146</v>
+        <v>148</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,9 +1456,8 @@
       <c r="B16" s="1">
         <v>153</v>
       </c>
-      <c r="C16" s="2">
-        <v>2</v>
-      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -1128,6 +1466,8 @@
       <c r="B17" s="1">
         <v>153</v>
       </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -1136,19 +1476,27 @@
       <c r="B18" s="1">
         <v>157</v>
       </c>
-      <c r="D18" s="2">
+      <c r="C18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="11"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="1">
         <v>158</v>
       </c>
-      <c r="D19" s="2">
+      <c r="C19" s="2">
         <v>1</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1158,82 +1506,98 @@
       <c r="B20" s="1">
         <v>166</v>
       </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="7">
+        <v>42172</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0</v>
       </c>
       <c r="B21" s="1">
-        <v>167</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" s="1">
-        <v>169</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>4</v>
+        <v>170</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1">
-        <v>170</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>0</v>
-      </c>
-      <c r="B24" s="3">
-        <v>171</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <v>128</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="7">
+        <v>42172</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="1">
-        <v>97</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>143</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1">
-        <v>114</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>10</v>
+        <v>167</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="1">
-        <v>160</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
+        <v>171</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="7">
+        <v>42172</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1241,17 +1605,104 @@
         <v>2</v>
       </c>
       <c r="B28" s="1">
+        <v>92</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>97</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
         <v>98</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="D30" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="7">
+        <v>42172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <v>114</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <v>135</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="7">
+        <v>42172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1">
+        <v>160</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="A2:E27">
-    <sortCondition ref="A2:A27"/>
-    <sortCondition ref="B2:B27"/>
+  <sortState ref="A2:E34">
+    <sortCondition ref="A2:A34"/>
+    <sortCondition ref="B2:B34"/>
   </sortState>
+  <conditionalFormatting sqref="A2:D33">
+    <cfRule type="expression" dxfId="37" priority="3">
+      <formula>$A2=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="4">
+      <formula>$A2=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="expression" dxfId="29" priority="1">
+      <formula>$A2=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="2">
+      <formula>$A2=2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>